<commit_message>
add with for answer
</commit_message>
<xml_diff>
--- a/ExportTemplates/questionTemplate.xlsx
+++ b/ExportTemplates/questionTemplate.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="SampleTestSet" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -145,9 +143,6 @@
     <t>Repeat Time</t>
   </si>
   <si>
-    <t>Online Test - Import Question</t>
-  </si>
-  <si>
     <t>File Name</t>
   </si>
   <si>
@@ -167,6 +162,9 @@
   </si>
   <si>
     <t>Answer 4</t>
+  </si>
+  <si>
+    <t>Online Test - Export Question</t>
   </si>
 </sst>
 </file>
@@ -295,49 +293,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="testset1.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="6600825" cy="8191500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -625,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:N5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -650,7 +605,7 @@
     <row r="1" spans="2:14" ht="11.25" customHeight="1"/>
     <row r="2" spans="2:14" ht="13.5" customHeight="1">
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -689,13 +644,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>5</v>
@@ -704,22 +659,22 @@
         <v>2</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -730,29 +685,4 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>